<commit_message>
Added new units to csv and fixed errors
</commit_message>
<xml_diff>
--- a/database/i18n/data/sheets/unit.xlsx
+++ b/database/i18n/data/sheets/unit.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drraf\Desktop\Appman\i18n\sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drraf\Documents\Privat\Development\Projects\appman-api-spec\database\i18n\data\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088D4869-AC4D-4936-80D7-D9828379240D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5068B831-FF68-4A4E-A37D-AC98C650830B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{270863C9-AB5C-4EC7-9F72-5036EBAD88B9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="331">
   <si>
     <t>unitID</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Square Millimeter</t>
   </si>
   <si>
-    <t>Square Mikrometer</t>
-  </si>
-  <si>
     <t>Square Nanometer</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>Gigabyte</t>
   </si>
   <si>
-    <t>Terrabyte</t>
-  </si>
-  <si>
     <t>Kibibyte</t>
   </si>
   <si>
@@ -150,9 +144,6 @@
     <t>Tebibyte</t>
   </si>
   <si>
-    <t>KB</t>
-  </si>
-  <si>
     <t>MB</t>
   </si>
   <si>
@@ -967,6 +958,75 @@
   </si>
   <si>
     <t>J/s</t>
+  </si>
+  <si>
+    <t>Square Micrometer</t>
+  </si>
+  <si>
+    <t>Kilobit</t>
+  </si>
+  <si>
+    <t>Megabit</t>
+  </si>
+  <si>
+    <t>Gigabit</t>
+  </si>
+  <si>
+    <t>Terabyte</t>
+  </si>
+  <si>
+    <t>Terabit</t>
+  </si>
+  <si>
+    <t>Kibibit</t>
+  </si>
+  <si>
+    <t>Mebibit</t>
+  </si>
+  <si>
+    <t>Gibibit</t>
+  </si>
+  <si>
+    <t>Tebibit</t>
+  </si>
+  <si>
+    <t>Mbit</t>
+  </si>
+  <si>
+    <t>Gbit</t>
+  </si>
+  <si>
+    <t>Tbit</t>
+  </si>
+  <si>
+    <t>Kibit</t>
+  </si>
+  <si>
+    <t>Mibit</t>
+  </si>
+  <si>
+    <t>Gibit</t>
+  </si>
+  <si>
+    <t>Tibit</t>
+  </si>
+  <si>
+    <t>Foot per Squaresecond</t>
+  </si>
+  <si>
+    <t>ft/s\u00B2</t>
+  </si>
+  <si>
+    <t>Kilonewton</t>
+  </si>
+  <si>
+    <t>kN</t>
+  </si>
+  <si>
+    <t>kbit</t>
+  </si>
+  <si>
+    <t>kB</t>
   </si>
 </sst>
 </file>
@@ -1404,10 +1464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B59370-60CF-4002-A2F9-A8D59013D45D}">
-  <dimension ref="A1:F155"/>
+  <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E120" sqref="E120"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,7 +1507,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D2" s="21">
         <v>1</v>
@@ -1468,7 +1528,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D3" s="19">
         <v>2.5399999999999999E-2</v>
@@ -1486,13 +1546,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>325</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>326</v>
       </c>
       <c r="D4" s="18">
-        <v>9.8066499999999994</v>
+        <v>0.30480000000000002</v>
       </c>
       <c r="E4" s="21">
         <v>0</v>
@@ -1507,19 +1567,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1.7453292519943198E-2</v>
+        <v>45</v>
+      </c>
+      <c r="D5" s="18">
+        <v>9.8066499999999994</v>
       </c>
       <c r="E5" s="21">
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1528,13 +1588,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="21">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1.7453292519943198E-2</v>
       </c>
       <c r="E6" s="21">
         <v>0</v>
@@ -1549,13 +1609,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D7" s="21">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E7" s="21">
         <v>0</v>
@@ -1570,19 +1630,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D8" s="21">
-        <v>1000000</v>
+        <v>0.9</v>
       </c>
       <c r="E8" s="21">
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1591,13 +1651,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D9" s="21">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="E9" s="21">
         <v>0</v>
@@ -1612,13 +1672,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="16">
-        <v>4046.8564224000002</v>
+        <v>61</v>
+      </c>
+      <c r="D10" s="21">
+        <v>100000</v>
       </c>
       <c r="E10" s="21">
         <v>0</v>
@@ -1633,13 +1693,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="21">
-        <v>100</v>
+        <v>62</v>
+      </c>
+      <c r="D11" s="16">
+        <v>4046.8564224000002</v>
       </c>
       <c r="E11" s="21">
         <v>0</v>
@@ -1654,13 +1714,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D12" s="21">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E12" s="21">
         <v>0</v>
@@ -1675,13 +1735,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="19">
-        <v>1E-4</v>
+        <v>52</v>
+      </c>
+      <c r="D13" s="21">
+        <v>1</v>
       </c>
       <c r="E13" s="21">
         <v>0</v>
@@ -1696,13 +1756,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="17">
-        <v>9.9999999999999995E-7</v>
+        <v>53</v>
+      </c>
+      <c r="D14" s="19">
+        <v>1E-4</v>
       </c>
       <c r="E14" s="21">
         <v>0</v>
@@ -1717,13 +1777,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="12">
-        <v>9.9999999999999998E-13</v>
+        <v>54</v>
+      </c>
+      <c r="D15" s="17">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E15" s="21">
         <v>0</v>
@@ -1738,13 +1798,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>308</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="8">
-        <v>1.0000000000000001E-18</v>
+        <v>56</v>
+      </c>
+      <c r="D16" s="12">
+        <v>9.9999999999999998E-13</v>
       </c>
       <c r="E16" s="21">
         <v>0</v>
@@ -1759,13 +1819,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="7">
-        <v>9.9999999999999995E-21</v>
+        <v>55</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1.0000000000000001E-18</v>
       </c>
       <c r="E17" s="21">
         <v>0</v>
@@ -1780,13 +1840,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="5">
-        <v>9.9999999999999992E-25</v>
+        <v>58</v>
+      </c>
+      <c r="D18" s="7">
+        <v>9.9999999999999995E-21</v>
       </c>
       <c r="E18" s="21">
         <v>0</v>
@@ -1801,13 +1861,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1.0000000000000001E-30</v>
+        <v>59</v>
+      </c>
+      <c r="D19" s="5">
+        <v>9.9999999999999992E-25</v>
       </c>
       <c r="E19" s="21">
         <v>0</v>
@@ -1822,13 +1882,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="15">
-        <v>6.4515999999999998E-4</v>
+        <v>60</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1.0000000000000001E-30</v>
       </c>
       <c r="E20" s="21">
         <v>0</v>
@@ -1843,13 +1903,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D21" s="15">
-        <v>9.2903040000000006E-2</v>
+        <v>6.4515999999999998E-4</v>
       </c>
       <c r="E21" s="21">
         <v>0</v>
@@ -1864,34 +1924,34 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="21">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="D22" s="15">
+        <v>9.2903040000000006E-2</v>
       </c>
       <c r="E22" s="21">
         <v>0</v>
       </c>
       <c r="F22" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <f t="shared" si="0"/>
+        <f>A22+1</f>
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D23" s="21">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E23" s="21">
         <v>0</v>
@@ -1906,14 +1966,14 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>309</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>38</v>
+        <v>329</v>
       </c>
       <c r="D24" s="21">
         <f>D23*1000</f>
-        <v>8000</v>
+        <v>1000</v>
       </c>
       <c r="E24" s="21">
         <v>0</v>
@@ -1928,14 +1988,14 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
+        <v>310</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>39</v>
+        <v>318</v>
       </c>
       <c r="D25" s="21">
-        <f t="shared" ref="D25:D27" si="1">D24*1000</f>
-        <v>8000000</v>
+        <f t="shared" ref="D25:D29" si="1">D24*1000</f>
+        <v>1000000</v>
       </c>
       <c r="E25" s="21">
         <v>0</v>
@@ -1950,14 +2010,14 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>311</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>40</v>
+        <v>319</v>
       </c>
       <c r="D26" s="21">
         <f t="shared" si="1"/>
-        <v>8000000000</v>
+        <v>1000000000</v>
       </c>
       <c r="E26" s="21">
         <v>0</v>
@@ -1972,14 +2032,14 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>33</v>
+        <v>313</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>41</v>
+        <v>320</v>
       </c>
       <c r="D27" s="21">
         <f t="shared" si="1"/>
-        <v>8000000000000</v>
+        <v>1000000000000</v>
       </c>
       <c r="E27" s="21">
         <v>0</v>
@@ -1994,14 +2054,14 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>314</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>42</v>
+        <v>321</v>
       </c>
       <c r="D28" s="21">
         <f>D23*1024</f>
-        <v>8192</v>
+        <v>1024</v>
       </c>
       <c r="E28" s="21">
         <v>0</v>
@@ -2016,14 +2076,14 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>35</v>
+        <v>315</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>43</v>
+        <v>322</v>
       </c>
       <c r="D29" s="21">
-        <f t="shared" ref="D29:D31" si="2">D24*1024</f>
-        <v>8192000</v>
+        <f>D28*1024</f>
+        <v>1048576</v>
       </c>
       <c r="E29" s="21">
         <v>0</v>
@@ -2038,14 +2098,14 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>316</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>44</v>
+        <v>323</v>
       </c>
       <c r="D30" s="21">
-        <f t="shared" si="2"/>
-        <v>8192000000</v>
+        <f t="shared" ref="D30:D32" si="2">D29*1024</f>
+        <v>1073741824</v>
       </c>
       <c r="E30" s="21">
         <v>0</v>
@@ -2060,14 +2120,14 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>317</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>45</v>
+        <v>324</v>
       </c>
       <c r="D31" s="21">
         <f t="shared" si="2"/>
-        <v>8192000000000</v>
+        <v>1099511627776</v>
       </c>
       <c r="E31" s="21">
         <v>0</v>
@@ -2082,19 +2142,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="6">
-        <v>1.6022000000000001E-19</v>
+        <v>28</v>
+      </c>
+      <c r="D32" s="21">
+        <v>8</v>
       </c>
       <c r="E32" s="21">
         <v>0</v>
       </c>
       <c r="F32" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2103,19 +2163,20 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>76</v>
+        <v>330</v>
       </c>
       <c r="D33" s="21">
-        <v>1</v>
+        <f>D32*1000</f>
+        <v>8000</v>
       </c>
       <c r="E33" s="21">
         <v>0</v>
       </c>
       <c r="F33" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2124,19 +2185,20 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="4">
-        <v>1E-3</v>
+        <v>36</v>
+      </c>
+      <c r="D34" s="21">
+        <f>D33*1000</f>
+        <v>8000000</v>
       </c>
       <c r="E34" s="21">
         <v>0</v>
       </c>
       <c r="F34" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2145,19 +2207,20 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="17">
-        <v>9.9999999999999995E-7</v>
+        <v>37</v>
+      </c>
+      <c r="D35" s="21">
+        <f>D34*1000</f>
+        <v>8000000000</v>
       </c>
       <c r="E35" s="21">
         <v>0</v>
       </c>
       <c r="F35" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2166,19 +2229,20 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>73</v>
+        <v>312</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>38</v>
+      </c>
+      <c r="D36" s="21">
+        <f>D35*1000</f>
+        <v>8000000000000</v>
       </c>
       <c r="E36" s="21">
         <v>0</v>
       </c>
       <c r="F36" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2187,19 +2251,20 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37" s="12">
-        <v>9.9999999999999998E-13</v>
+        <v>39</v>
+      </c>
+      <c r="D37" s="21">
+        <f>D32*1024</f>
+        <v>8192</v>
       </c>
       <c r="E37" s="21">
         <v>0</v>
       </c>
       <c r="F37" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2208,19 +2273,20 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="D38" s="21">
-        <v>1000</v>
+        <f>D37*1024</f>
+        <v>8388608</v>
       </c>
       <c r="E38" s="21">
         <v>0</v>
       </c>
       <c r="F38" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2229,19 +2295,20 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="D39" s="21">
-        <v>1</v>
+        <f t="shared" ref="D39:D40" si="3">D38*1024</f>
+        <v>8589934592</v>
       </c>
       <c r="E39" s="21">
         <v>0</v>
       </c>
       <c r="F39" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2250,19 +2317,20 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D40" s="4">
-        <v>1E-3</v>
+        <v>42</v>
+      </c>
+      <c r="D40" s="21">
+        <f>D39*1024</f>
+        <v>8796093022208</v>
       </c>
       <c r="E40" s="21">
         <v>0</v>
       </c>
       <c r="F40" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2271,19 +2339,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D41" s="17">
-        <v>9.9999999999999995E-7</v>
+        <v>72</v>
+      </c>
+      <c r="D41" s="6">
+        <v>1.6022000000000001E-19</v>
       </c>
       <c r="E41" s="21">
         <v>0</v>
       </c>
       <c r="F41" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2292,19 +2360,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D42" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>73</v>
+      </c>
+      <c r="D42" s="21">
+        <v>1</v>
       </c>
       <c r="E42" s="21">
         <v>0</v>
       </c>
       <c r="F42" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2313,19 +2381,19 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" s="12">
-        <v>9.9999999999999998E-13</v>
+        <v>74</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1E-3</v>
       </c>
       <c r="E43" s="21">
         <v>0</v>
       </c>
       <c r="F43" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2334,19 +2402,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D44" s="4">
-        <v>1E-3</v>
+        <v>75</v>
+      </c>
+      <c r="D44" s="17">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E44" s="21">
         <v>0</v>
       </c>
       <c r="F44" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2355,19 +2423,19 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D45" s="21">
-        <v>1</v>
+        <v>76</v>
+      </c>
+      <c r="D45" s="14">
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="E45" s="21">
         <v>0</v>
       </c>
       <c r="F45" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2376,19 +2444,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D46" s="21">
-        <v>1000</v>
+        <v>77</v>
+      </c>
+      <c r="D46" s="12">
+        <v>9.9999999999999998E-13</v>
       </c>
       <c r="E46" s="21">
         <v>0</v>
       </c>
       <c r="F46" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2397,19 +2465,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="D47" s="21">
-        <v>1000000</v>
+        <v>1000</v>
       </c>
       <c r="E47" s="21">
         <v>0</v>
       </c>
       <c r="F47" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2418,19 +2486,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D48" s="19">
-        <v>4.1867999999999999</v>
+        <v>85</v>
+      </c>
+      <c r="D48" s="21">
+        <v>1</v>
       </c>
       <c r="E48" s="21">
         <v>0</v>
       </c>
       <c r="F48" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2439,19 +2507,19 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D49" s="21">
-        <v>4186.8</v>
+        <v>86</v>
+      </c>
+      <c r="D49" s="4">
+        <v>1E-3</v>
       </c>
       <c r="E49" s="21">
         <v>0</v>
       </c>
       <c r="F49" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2460,19 +2528,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50" s="21">
-        <v>1</v>
+        <v>87</v>
+      </c>
+      <c r="D50" s="17">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E50" s="21">
         <v>0</v>
       </c>
       <c r="F50" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2481,19 +2549,19 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D51" s="21">
-        <v>3600</v>
+        <v>88</v>
+      </c>
+      <c r="D51" s="14">
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="E51" s="21">
         <v>0</v>
       </c>
       <c r="F51" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2502,19 +2570,19 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D52" s="21">
-        <v>1000</v>
+        <v>89</v>
+      </c>
+      <c r="D52" s="12">
+        <v>9.9999999999999998E-13</v>
       </c>
       <c r="E52" s="21">
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2523,13 +2591,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D53" s="21">
-        <v>3600000</v>
+        <v>100</v>
+      </c>
+      <c r="D53" s="4">
+        <v>1E-3</v>
       </c>
       <c r="E53" s="21">
         <v>0</v>
@@ -2544,10 +2612,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D54" s="21">
         <v>1</v>
@@ -2556,7 +2624,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2565,19 +2633,19 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D55" s="18">
-        <v>9.8066499999999994</v>
+        <v>102</v>
+      </c>
+      <c r="D55" s="21">
+        <v>1000</v>
       </c>
       <c r="E55" s="21">
         <v>0</v>
       </c>
       <c r="F55" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2586,19 +2654,19 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D56" s="13">
-        <v>4.4482216152999996</v>
+        <v>103</v>
+      </c>
+      <c r="D56" s="21">
+        <v>1000000</v>
       </c>
       <c r="E56" s="21">
         <v>0</v>
       </c>
       <c r="F56" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2607,19 +2675,19 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D57" s="21">
-        <v>1000</v>
+        <v>104</v>
+      </c>
+      <c r="D57" s="19">
+        <v>4.1867999999999999</v>
       </c>
       <c r="E57" s="21">
         <v>0</v>
       </c>
       <c r="F57" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2628,19 +2696,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="D58" s="21">
-        <v>100</v>
+        <v>4186.8</v>
       </c>
       <c r="E58" s="21">
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2649,10 +2717,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="D59" s="21">
         <v>1</v>
@@ -2661,7 +2729,7 @@
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2670,19 +2738,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="D60" s="21">
-        <v>0.1</v>
+        <v>3600</v>
       </c>
       <c r="E60" s="21">
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2691,19 +2759,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D61" s="20">
-        <v>0.01</v>
+        <v>108</v>
+      </c>
+      <c r="D61" s="21">
+        <v>1000</v>
       </c>
       <c r="E61" s="21">
         <v>0</v>
       </c>
       <c r="F61" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2712,19 +2780,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D62" s="4">
-        <v>1E-3</v>
+        <v>109</v>
+      </c>
+      <c r="D62" s="21">
+        <v>3600000</v>
       </c>
       <c r="E62" s="21">
         <v>0</v>
       </c>
       <c r="F62" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2733,19 +2801,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>127</v>
+        <v>327</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D63" s="17">
-        <v>9.9999999999999995E-7</v>
+        <v>328</v>
+      </c>
+      <c r="D63" s="21">
+        <v>1000</v>
       </c>
       <c r="E63" s="21">
         <v>0</v>
       </c>
       <c r="F63" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2754,19 +2822,19 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D64" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>111</v>
+      </c>
+      <c r="D64" s="21">
+        <v>1</v>
       </c>
       <c r="E64" s="21">
         <v>0</v>
       </c>
       <c r="F64" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2775,19 +2843,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D65" s="13">
-        <v>1E-10</v>
+        <v>112</v>
+      </c>
+      <c r="D65" s="18">
+        <v>9.8066499999999994</v>
       </c>
       <c r="E65" s="21">
         <v>0</v>
       </c>
       <c r="F65" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2796,19 +2864,19 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D66" s="12">
-        <v>9.9999999999999998E-13</v>
+        <v>113</v>
+      </c>
+      <c r="D66" s="13">
+        <v>4.4482216152999996</v>
       </c>
       <c r="E66" s="21">
         <v>0</v>
       </c>
       <c r="F66" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2817,13 +2885,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D67" s="10">
-        <v>1.0000000000000001E-15</v>
+        <v>49</v>
+      </c>
+      <c r="D67" s="21">
+        <v>1000</v>
       </c>
       <c r="E67" s="21">
         <v>0</v>
@@ -2834,17 +2902,17 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <f t="shared" ref="A68:A131" si="3">A67+1</f>
+        <f t="shared" ref="A68:A131" si="4">A67+1</f>
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D68" s="19">
-        <v>2.5399999999999999E-2</v>
+        <v>117</v>
+      </c>
+      <c r="D68" s="21">
+        <v>100</v>
       </c>
       <c r="E68" s="21">
         <v>0</v>
@@ -2855,17 +2923,17 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D69" s="4">
-        <v>1609.3440000000001</v>
+        <v>51</v>
+      </c>
+      <c r="D69" s="21">
+        <v>1</v>
       </c>
       <c r="E69" s="21">
         <v>0</v>
@@ -2876,17 +2944,17 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="D70" s="21">
-        <v>1852</v>
+        <v>0.1</v>
       </c>
       <c r="E70" s="21">
         <v>0</v>
@@ -2897,17 +2965,17 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D71" s="18">
-        <v>0.30480000000000002</v>
+        <v>121</v>
+      </c>
+      <c r="D71" s="20">
+        <v>0.01</v>
       </c>
       <c r="E71" s="21">
         <v>0</v>
@@ -2918,17 +2986,17 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D72" s="18">
-        <v>0.91439999999999999</v>
+        <v>123</v>
+      </c>
+      <c r="D72" s="4">
+        <v>1E-3</v>
       </c>
       <c r="E72" s="21">
         <v>0</v>
@@ -2939,17 +3007,17 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D73" s="21">
-        <v>9460730000000000</v>
+        <v>125</v>
+      </c>
+      <c r="D73" s="17">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E73" s="21">
         <v>0</v>
@@ -2960,17 +3028,17 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D74" s="21">
-        <v>3.085678E+16</v>
+        <v>130</v>
+      </c>
+      <c r="D74" s="14">
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="E74" s="21">
         <v>0</v>
@@ -2981,17 +3049,17 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D75" s="14">
-        <v>2.6458299999999998E-4</v>
+        <v>57</v>
+      </c>
+      <c r="D75" s="13">
+        <v>1E-10</v>
       </c>
       <c r="E75" s="21">
         <v>0</v>
@@ -3002,17 +3070,17 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D76" s="13">
-        <v>3.5277779999999998E-4</v>
+        <v>131</v>
+      </c>
+      <c r="D76" s="12">
+        <v>9.9999999999999998E-13</v>
       </c>
       <c r="E76" s="21">
         <v>0</v>
@@ -3023,17 +3091,17 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D77" s="13">
-        <v>4.2333333000000003E-3</v>
+        <v>132</v>
+      </c>
+      <c r="D77" s="10">
+        <v>1.0000000000000001E-15</v>
       </c>
       <c r="E77" s="21">
         <v>0</v>
@@ -3044,17 +3112,17 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D78" s="13">
-        <v>4.2175175999999998E-3</v>
+        <v>146</v>
+      </c>
+      <c r="D78" s="19">
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="E78" s="21">
         <v>0</v>
@@ -3065,455 +3133,455 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D79" s="21">
-        <v>1</v>
+        <v>147</v>
+      </c>
+      <c r="D79" s="4">
+        <v>1609.3440000000001</v>
       </c>
       <c r="E79" s="21">
         <v>0</v>
       </c>
       <c r="F79" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D80" s="21">
-        <v>10000</v>
+        <v>1852</v>
       </c>
       <c r="E80" s="21">
         <v>0</v>
       </c>
       <c r="F80" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D81" s="19">
-        <v>1550.0030999999999</v>
+        <v>149</v>
+      </c>
+      <c r="D81" s="18">
+        <v>0.30480000000000002</v>
       </c>
       <c r="E81" s="21">
         <v>0</v>
       </c>
       <c r="F81" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D82" s="13">
-        <v>10.7639104167</v>
+        <v>150</v>
+      </c>
+      <c r="D82" s="18">
+        <v>0.91439999999999999</v>
       </c>
       <c r="E82" s="21">
         <v>0</v>
       </c>
       <c r="F82" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D83" s="15">
-        <v>3183.0988618299998</v>
+        <v>151</v>
+      </c>
+      <c r="D83" s="21">
+        <v>9460730000000000</v>
       </c>
       <c r="E83" s="21">
         <v>0</v>
       </c>
       <c r="F83" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D84" s="13">
-        <v>3.4262590996000002</v>
+        <v>152</v>
+      </c>
+      <c r="D84" s="21">
+        <v>3.085678E+16</v>
       </c>
       <c r="E84" s="21">
         <v>0</v>
       </c>
       <c r="F84" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D85" s="21">
-        <v>1</v>
+        <v>153</v>
+      </c>
+      <c r="D85" s="14">
+        <v>2.6458299999999998E-4</v>
       </c>
       <c r="E85" s="21">
         <v>0</v>
       </c>
       <c r="F85" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D86" s="21">
-        <v>10000</v>
+        <v>154</v>
+      </c>
+      <c r="D86" s="13">
+        <v>3.5277779999999998E-4</v>
       </c>
       <c r="E86" s="21">
         <v>0</v>
       </c>
       <c r="F86" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="D87" s="13">
-        <v>10.7639104167</v>
+        <v>4.2333333000000003E-3</v>
       </c>
       <c r="E87" s="21">
         <v>0</v>
       </c>
       <c r="F87" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D88" s="19">
-        <v>1550.0030999999999</v>
+        <v>156</v>
+      </c>
+      <c r="D88" s="13">
+        <v>4.2175175999999998E-3</v>
       </c>
       <c r="E88" s="21">
         <v>0</v>
       </c>
       <c r="F88" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>190</v>
+        <v>158</v>
       </c>
       <c r="D89" s="21">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="E89" s="21">
         <v>0</v>
       </c>
       <c r="F89" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>191</v>
+        <v>160</v>
       </c>
       <c r="D90" s="21">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="E90" s="21">
         <v>0</v>
       </c>
       <c r="F90" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D91" s="4">
-        <v>1E-3</v>
+        <v>162</v>
+      </c>
+      <c r="D91" s="19">
+        <v>1550.0030999999999</v>
       </c>
       <c r="E91" s="21">
         <v>0</v>
       </c>
       <c r="F91" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D92" s="17">
-        <v>9.9999999999999995E-7</v>
+        <v>164</v>
+      </c>
+      <c r="D92" s="13">
+        <v>10.7639104167</v>
       </c>
       <c r="E92" s="21">
         <v>0</v>
       </c>
       <c r="F92" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D93" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>167</v>
+      </c>
+      <c r="D93" s="15">
+        <v>3183.0988618299998</v>
       </c>
       <c r="E93" s="21">
         <v>0</v>
       </c>
       <c r="F93" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D94" s="12">
-        <v>9.9999999999999998E-13</v>
+        <v>168</v>
+      </c>
+      <c r="D94" s="13">
+        <v>3.4262590996000002</v>
       </c>
       <c r="E94" s="21">
         <v>0</v>
       </c>
       <c r="F94" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D95" s="10">
-        <v>1.0000000000000001E-15</v>
+        <v>173</v>
+      </c>
+      <c r="D95" s="21">
+        <v>1</v>
       </c>
       <c r="E95" s="21">
         <v>0</v>
       </c>
       <c r="F95" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D96" s="8">
-        <v>1.0000000000000001E-18</v>
+        <v>174</v>
+      </c>
+      <c r="D96" s="21">
+        <v>10000</v>
       </c>
       <c r="E96" s="21">
         <v>0</v>
       </c>
       <c r="F96" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D97" s="4">
-        <v>2.8000000000000001E-2</v>
+        <v>175</v>
+      </c>
+      <c r="D97" s="13">
+        <v>10.7639104167</v>
       </c>
       <c r="E97" s="21">
         <v>0</v>
       </c>
       <c r="F97" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D98" s="15">
-        <v>0.45359237000000002</v>
+        <v>176</v>
+      </c>
+      <c r="D98" s="19">
+        <v>1550.0030999999999</v>
       </c>
       <c r="E98" s="21">
         <v>0</v>
       </c>
       <c r="F98" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D99" s="4">
-        <v>1E-3</v>
+        <v>187</v>
+      </c>
+      <c r="D99" s="21">
+        <v>1000</v>
       </c>
       <c r="E99" s="21">
         <v>0</v>
       </c>
       <c r="F99" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="D100" s="21">
         <v>1</v>
@@ -3522,229 +3590,229 @@
         <v>0</v>
       </c>
       <c r="F100" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D101" s="21">
-        <v>100</v>
+        <v>45</v>
+      </c>
+      <c r="D101" s="4">
+        <v>1E-3</v>
       </c>
       <c r="E101" s="21">
         <v>0</v>
       </c>
       <c r="F101" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D102" s="21">
-        <v>1000</v>
+        <v>189</v>
+      </c>
+      <c r="D102" s="17">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E102" s="21">
         <v>0</v>
       </c>
       <c r="F102" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D103" s="21">
-        <v>100000</v>
+        <v>190</v>
+      </c>
+      <c r="D103" s="14">
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="E103" s="21">
         <v>0</v>
       </c>
       <c r="F103" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D104" s="21">
-        <v>100</v>
+        <v>191</v>
+      </c>
+      <c r="D104" s="12">
+        <v>9.9999999999999998E-13</v>
       </c>
       <c r="E104" s="21">
         <v>0</v>
       </c>
       <c r="F104" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D105" s="14">
-        <v>133.32236842099999</v>
+        <v>192</v>
+      </c>
+      <c r="D105" s="10">
+        <v>1.0000000000000001E-15</v>
       </c>
       <c r="E105" s="21">
         <v>0</v>
       </c>
       <c r="F105" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D106" s="14">
-        <v>6894.7572931779996</v>
+        <v>193</v>
+      </c>
+      <c r="D106" s="8">
+        <v>1.0000000000000001E-18</v>
       </c>
       <c r="E106" s="21">
         <v>0</v>
       </c>
       <c r="F106" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D107" s="18">
-        <v>47.88026</v>
+        <v>194</v>
+      </c>
+      <c r="D107" s="4">
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="E107" s="21">
         <v>0</v>
       </c>
       <c r="F107" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D108" s="21">
-        <v>101325</v>
+        <v>195</v>
+      </c>
+      <c r="D108" s="15">
+        <v>0.45359237000000002</v>
       </c>
       <c r="E108" s="21">
         <v>0</v>
       </c>
       <c r="F108" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D109" s="21">
-        <v>1</v>
+        <v>206</v>
+      </c>
+      <c r="D109" s="4">
+        <v>1E-3</v>
       </c>
       <c r="E109" s="21">
         <v>0</v>
       </c>
       <c r="F109" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D110" s="21">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E110" s="21">
         <v>0</v>
       </c>
       <c r="F110" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="D111" s="21">
         <v>100</v>
@@ -3753,112 +3821,112 @@
         <v>0</v>
       </c>
       <c r="F111" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>111</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D112" s="4">
-        <v>1E-3</v>
+        <v>209</v>
+      </c>
+      <c r="D112" s="21">
+        <v>1000</v>
       </c>
       <c r="E112" s="21">
         <v>0</v>
       </c>
       <c r="F112" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="D113" s="21">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="E113" s="21">
         <v>0</v>
       </c>
       <c r="F113" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D114" s="13">
-        <v>0.27777777780000001</v>
+        <v>211</v>
+      </c>
+      <c r="D114" s="21">
+        <v>100</v>
       </c>
       <c r="E114" s="21">
         <v>0</v>
       </c>
       <c r="F114" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>114</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D115" s="13">
-        <v>0.4472271914</v>
+        <v>202</v>
+      </c>
+      <c r="D115" s="14">
+        <v>133.32236842099999</v>
       </c>
       <c r="E115" s="21">
         <v>0</v>
       </c>
       <c r="F115" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>115</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D116" s="11">
-        <v>0.51444444444444004</v>
+        <v>212</v>
+      </c>
+      <c r="D116" s="14">
+        <v>6894.7572931779996</v>
       </c>
       <c r="E116" s="21">
         <v>0</v>
       </c>
       <c r="F116" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3867,808 +3935,808 @@
         <v>116</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D117" s="11">
-        <v>2.9386699579699999E-3</v>
+        <v>213</v>
+      </c>
+      <c r="D117" s="18">
+        <v>47.88026</v>
       </c>
       <c r="E117" s="21">
         <v>0</v>
       </c>
       <c r="F117" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>117</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>237</v>
+        <v>214</v>
       </c>
       <c r="D118" s="21">
-        <v>1</v>
+        <v>101325</v>
       </c>
       <c r="E118" s="21">
         <v>0</v>
       </c>
       <c r="F118" s="1">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>118</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="D119" s="21">
         <v>1</v>
       </c>
-      <c r="E119" s="4">
-        <v>273.14999999999998</v>
+      <c r="E119" s="21">
+        <v>0</v>
       </c>
       <c r="F119" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>119</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D120" s="10">
-        <v>0.55555555555555503</v>
-      </c>
-      <c r="E120" s="4">
-        <v>459.67</v>
+        <v>218</v>
+      </c>
+      <c r="D120" s="21">
+        <v>10</v>
+      </c>
+      <c r="E120" s="21">
+        <v>0</v>
       </c>
       <c r="F120" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="D121" s="21">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E121" s="21">
         <v>0</v>
       </c>
       <c r="F121" s="1">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>121</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>243</v>
+        <v>221</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D122" s="14">
-        <v>0.16666666699999999</v>
+        <v>227</v>
+      </c>
+      <c r="D122" s="4">
+        <v>1E-3</v>
       </c>
       <c r="E122" s="21">
         <v>0</v>
       </c>
       <c r="F122" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>122</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>244</v>
+        <v>222</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D123" s="13">
-        <v>2.777778E-4</v>
+        <v>228</v>
+      </c>
+      <c r="D123" s="21">
+        <v>1</v>
       </c>
       <c r="E123" s="21">
         <v>0</v>
       </c>
       <c r="F123" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>123</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D124" s="21">
-        <v>604800</v>
+        <v>229</v>
+      </c>
+      <c r="D124" s="13">
+        <v>0.27777777780000001</v>
       </c>
       <c r="E124" s="21">
         <v>0</v>
       </c>
       <c r="F124" s="1">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>124</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="D125" s="21">
-        <v>86400</v>
+        <v>230</v>
+      </c>
+      <c r="D125" s="13">
+        <v>0.4472271914</v>
       </c>
       <c r="E125" s="21">
         <v>0</v>
       </c>
       <c r="F125" s="1">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>125</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D126" s="21">
-        <v>3600</v>
+        <v>231</v>
+      </c>
+      <c r="D126" s="11">
+        <v>0.51444444444444004</v>
       </c>
       <c r="E126" s="21">
         <v>0</v>
       </c>
       <c r="F126" s="1">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>126</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D127" s="21">
-        <v>60</v>
+        <v>232</v>
+      </c>
+      <c r="D127" s="11">
+        <v>2.9386699579699999E-3</v>
       </c>
       <c r="E127" s="21">
         <v>0</v>
       </c>
       <c r="F127" s="1">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>127</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="D128" s="22">
+        <v>234</v>
+      </c>
+      <c r="D128" s="21">
         <v>1</v>
       </c>
       <c r="E128" s="21">
         <v>0</v>
       </c>
       <c r="F128" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>128</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D129" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="E129" s="21">
-        <v>0</v>
+        <v>237</v>
+      </c>
+      <c r="D129" s="21">
+        <v>1</v>
+      </c>
+      <c r="E129" s="4">
+        <v>273.14999999999998</v>
       </c>
       <c r="F129" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>129</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="D130" s="17">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="E130" s="21">
-        <v>0</v>
+        <v>238</v>
+      </c>
+      <c r="D130" s="10">
+        <v>0.55555555555555503</v>
+      </c>
+      <c r="E130" s="4">
+        <v>459.67</v>
       </c>
       <c r="F130" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>130</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D131" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>242</v>
+      </c>
+      <c r="D131" s="21">
+        <v>1</v>
       </c>
       <c r="E131" s="21">
         <v>0</v>
       </c>
       <c r="F131" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <f t="shared" ref="A132:A155" si="4">A131+1</f>
+        <f t="shared" ref="A132:A165" si="5">A131+1</f>
         <v>131</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D132" s="12">
-        <v>9.9999999999999998E-13</v>
+        <v>243</v>
+      </c>
+      <c r="D132" s="14">
+        <v>0.16666666699999999</v>
       </c>
       <c r="E132" s="21">
         <v>0</v>
       </c>
       <c r="F132" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>132</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="D133" s="10">
-        <v>1.0000000000000001E-15</v>
+        <v>244</v>
+      </c>
+      <c r="D133" s="13">
+        <v>2.777778E-4</v>
       </c>
       <c r="E133" s="21">
         <v>0</v>
       </c>
       <c r="F133" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>133</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="D134" s="21">
-        <v>1</v>
+        <v>604800</v>
       </c>
       <c r="E134" s="21">
         <v>0</v>
       </c>
       <c r="F134" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>134</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D135" s="14">
-        <v>0.101971621</v>
+        <v>256</v>
+      </c>
+      <c r="D135" s="21">
+        <v>86400</v>
       </c>
       <c r="E135" s="21">
         <v>0</v>
       </c>
       <c r="F135" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>135</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D136" s="13">
-        <v>1.3358179482999999</v>
+        <v>257</v>
+      </c>
+      <c r="D136" s="21">
+        <v>3600</v>
       </c>
       <c r="E136" s="21">
         <v>0</v>
       </c>
       <c r="F136" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>136</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D137" s="14">
-        <v>0.11298482899999999</v>
+        <v>51</v>
+      </c>
+      <c r="D137" s="21">
+        <v>60</v>
       </c>
       <c r="E137" s="21">
         <v>0</v>
       </c>
       <c r="F137" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>137</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>275</v>
+        <v>249</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D138" s="4">
-        <v>1E-3</v>
+        <v>258</v>
+      </c>
+      <c r="D138" s="22">
+        <v>1</v>
       </c>
       <c r="E138" s="21">
         <v>0</v>
       </c>
       <c r="F138" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>138</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>276</v>
+        <v>250</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D139" s="21">
-        <v>1</v>
+        <v>259</v>
+      </c>
+      <c r="D139" s="4">
+        <v>1E-3</v>
       </c>
       <c r="E139" s="21">
         <v>0</v>
       </c>
       <c r="F139" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>139</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D140" s="21">
-        <v>1000</v>
+        <v>260</v>
+      </c>
+      <c r="D140" s="17">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E140" s="21">
         <v>0</v>
       </c>
       <c r="F140" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>140</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>278</v>
+        <v>252</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D141" s="21">
-        <v>1000000</v>
+        <v>261</v>
+      </c>
+      <c r="D141" s="14">
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="E141" s="21">
         <v>0</v>
       </c>
       <c r="F141" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>141</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>283</v>
+        <v>253</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="D142" s="14">
-        <v>1.0000000000000001E-9</v>
+        <v>262</v>
+      </c>
+      <c r="D142" s="12">
+        <v>9.9999999999999998E-13</v>
       </c>
       <c r="E142" s="21">
         <v>0</v>
       </c>
       <c r="F142" s="1">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>142</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>284</v>
+        <v>254</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D143" s="17">
-        <v>9.9999999999999995E-7</v>
+        <v>263</v>
+      </c>
+      <c r="D143" s="10">
+        <v>1.0000000000000001E-15</v>
       </c>
       <c r="E143" s="21">
         <v>0</v>
       </c>
       <c r="F143" s="1">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>143</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D144" s="4">
-        <v>1E-3</v>
+        <v>268</v>
+      </c>
+      <c r="D144" s="21">
+        <v>1</v>
       </c>
       <c r="E144" s="21">
         <v>0</v>
       </c>
       <c r="F144" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>144</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D145" s="21">
-        <v>1</v>
+        <v>269</v>
+      </c>
+      <c r="D145" s="14">
+        <v>0.101971621</v>
       </c>
       <c r="E145" s="21">
         <v>0</v>
       </c>
       <c r="F145" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>145</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
       <c r="D146" s="13">
-        <v>3.7854118000000001E-3</v>
+        <v>1.3358179482999999</v>
       </c>
       <c r="E146" s="21">
         <v>0</v>
       </c>
       <c r="F146" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>146</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="D147" s="13">
-        <v>2.8316846600000001E-2</v>
+        <v>271</v>
+      </c>
+      <c r="D147" s="14">
+        <v>0.11298482899999999</v>
       </c>
       <c r="E147" s="21">
         <v>0</v>
       </c>
       <c r="F147" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>147</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D148" s="13">
-        <v>1.6387100000000001E-5</v>
+        <v>276</v>
+      </c>
+      <c r="D148" s="4">
+        <v>1E-3</v>
       </c>
       <c r="E148" s="21">
         <v>0</v>
       </c>
       <c r="F148" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>148</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>297</v>
+        <v>273</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="D149" s="4">
-        <v>1E-3</v>
+        <v>277</v>
+      </c>
+      <c r="D149" s="21">
+        <v>1</v>
       </c>
       <c r="E149" s="21">
         <v>0</v>
       </c>
       <c r="F149" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>149</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>304</v>
+        <v>278</v>
       </c>
       <c r="D150" s="21">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="E150" s="21">
         <v>0</v>
       </c>
       <c r="F150" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>306</v>
+        <v>279</v>
       </c>
       <c r="D151" s="21">
-        <v>1000</v>
+        <v>1000000</v>
       </c>
       <c r="E151" s="21">
         <v>0</v>
       </c>
       <c r="F151" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>151</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="D152" s="21">
-        <v>1000000</v>
+        <v>287</v>
+      </c>
+      <c r="D152" s="14">
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="E152" s="21">
         <v>0</v>
       </c>
       <c r="F152" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>152</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="D153" s="21">
-        <v>1000000000</v>
+        <v>288</v>
+      </c>
+      <c r="D153" s="17">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E153" s="21">
         <v>0</v>
       </c>
       <c r="F153" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>153</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="D154" s="18">
-        <v>735.49874999999997</v>
+        <v>289</v>
+      </c>
+      <c r="D154" s="4">
+        <v>1E-3</v>
       </c>
       <c r="E154" s="21">
         <v>0</v>
       </c>
       <c r="F154" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>154</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="D155" s="21">
         <v>1</v>
@@ -4677,6 +4745,216 @@
         <v>0</v>
       </c>
       <c r="F155" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <f t="shared" si="5"/>
+        <v>155</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D156" s="13">
+        <v>3.7854118000000001E-3</v>
+      </c>
+      <c r="E156" s="21">
+        <v>0</v>
+      </c>
+      <c r="F156" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <f t="shared" si="5"/>
+        <v>156</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D157" s="13">
+        <v>2.8316846600000001E-2</v>
+      </c>
+      <c r="E157" s="21">
+        <v>0</v>
+      </c>
+      <c r="F157" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <f t="shared" si="5"/>
+        <v>157</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D158" s="13">
+        <v>1.6387100000000001E-5</v>
+      </c>
+      <c r="E158" s="21">
+        <v>0</v>
+      </c>
+      <c r="F158" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <f t="shared" si="5"/>
+        <v>158</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D159" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="E159" s="21">
+        <v>0</v>
+      </c>
+      <c r="F159" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <f t="shared" si="5"/>
+        <v>159</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D160" s="21">
+        <v>1</v>
+      </c>
+      <c r="E160" s="21">
+        <v>0</v>
+      </c>
+      <c r="F160" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <f t="shared" si="5"/>
+        <v>160</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D161" s="21">
+        <v>1000</v>
+      </c>
+      <c r="E161" s="21">
+        <v>0</v>
+      </c>
+      <c r="F161" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <f t="shared" si="5"/>
+        <v>161</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D162" s="21">
+        <v>1000000</v>
+      </c>
+      <c r="E162" s="21">
+        <v>0</v>
+      </c>
+      <c r="F162" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <f t="shared" si="5"/>
+        <v>162</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D163" s="21">
+        <v>1000000000</v>
+      </c>
+      <c r="E163" s="21">
+        <v>0</v>
+      </c>
+      <c r="F163" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <f t="shared" si="5"/>
+        <v>163</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D164" s="18">
+        <v>735.49874999999997</v>
+      </c>
+      <c r="E164" s="21">
+        <v>0</v>
+      </c>
+      <c r="F164" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <f t="shared" si="5"/>
+        <v>164</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D165" s="21">
+        <v>1</v>
+      </c>
+      <c r="E165" s="21">
+        <v>0</v>
+      </c>
+      <c r="F165" s="1">
         <v>22</v>
       </c>
     </row>

</xml_diff>